<commit_message>
test(weighted_mean): add sum_weights column to test
</commit_message>
<xml_diff>
--- a/tests/test-data/weighted-mean-inputs.xlsx
+++ b/tests/test-data/weighted-mean-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\household-size\tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE0E635-D584-44B3-BED3-75159DB14267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD39A90E-010C-4F95-8260-42B42382918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17520" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5630" yWindow="160" windowWidth="11300" windowHeight="14090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>HHINCOME_bucket</t>
   </si>
@@ -99,6 +99,39 @@
   </si>
   <si>
     <t>weighted_mean</t>
+  </si>
+  <si>
+    <t>sum_weights</t>
+  </si>
+  <si>
+    <t>r000_100k</t>
+  </si>
+  <si>
+    <t>r00_49</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>r50plus</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>r100kplus</t>
+  </si>
+  <si>
+    <t>aapi</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>hispanic</t>
+  </si>
+  <si>
+    <t>aian</t>
   </si>
 </sst>
 </file>
@@ -293,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -301,12 +334,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -316,21 +348,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,23 +642,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="22.140625" customWidth="1"/>
+    <col min="1" max="6" width="22.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -650,7 +682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -669,44 +701,44 @@
       <c r="F3" s="4">
         <v>39</v>
       </c>
-      <c r="G3" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="G3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="11">
+        <v>2</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>30</v>
       </c>
-      <c r="G4" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>2</v>
       </c>
       <c r="E5" s="5">
@@ -715,21 +747,21 @@
       <c r="F5" s="6">
         <v>71</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="27">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
       <c r="E6" s="3">
@@ -738,90 +770,90 @@
       <c r="F6" s="4">
         <v>50</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>35</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="22">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="21">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>41</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="22">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="21">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>42</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="25">
         <v>2</v>
       </c>
       <c r="E10" s="5">
@@ -830,67 +862,67 @@
       <c r="F10" s="6">
         <v>60</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="30">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9">
-        <v>1</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="D11" s="29">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
         <v>13</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="29">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="14">
-        <v>2</v>
-      </c>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10">
+      <c r="D12" s="13">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
         <v>43</v>
       </c>
-      <c r="G12" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="G12" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>2</v>
       </c>
       <c r="E13" s="3">
@@ -899,21 +931,21 @@
       <c r="F13" s="4">
         <v>65</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="34">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>2</v>
       </c>
       <c r="E14" s="5">
@@ -922,34 +954,34 @@
       <c r="F14" s="6">
         <v>45</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="27">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="32">
-        <v>2</v>
-      </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="D15" s="31">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
         <v>34</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="34">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -968,21 +1000,21 @@
       <c r="F16" s="4">
         <v>26</v>
       </c>
-      <c r="G16" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="G16" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <v>2</v>
       </c>
       <c r="E17" s="5">
@@ -991,16 +1023,16 @@
       <c r="F17" s="6">
         <v>33</v>
       </c>
-      <c r="G17" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1020,18 +1052,21 @@
         <v>20</v>
       </c>
       <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1043,21 +1078,25 @@
         <f>(E3*F3+E16*F16)/(F3+F16)</f>
         <v>2.6</v>
       </c>
-      <c r="G21" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="12">
+      <c r="G21">
+        <f>F3+F16</f>
+        <v>65</v>
+      </c>
+      <c r="H21" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="11">
         <v>2</v>
       </c>
       <c r="E22">
@@ -1067,21 +1106,25 @@
         <f>(E4*F4+E12*F12+E17*F17)/(F4+F12+F17)</f>
         <v>1.8773584905660377</v>
       </c>
-      <c r="G22" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="18">
+      <c r="G22">
+        <f>F4+F12+F17</f>
+        <v>106</v>
+      </c>
+      <c r="H22" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="17">
         <v>2</v>
       </c>
       <c r="E23">
@@ -1091,21 +1134,25 @@
         <f>(E5*F5+E14*F14)/(F5+F14)</f>
         <v>2.6120689655172415</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G23">
+        <f>F5+F14</f>
+        <v>116</v>
+      </c>
+      <c r="H23" s="27">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="20">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="19">
         <v>1</v>
       </c>
       <c r="E24">
@@ -1115,21 +1162,25 @@
         <f>(E6*F6+E8*F8+E9*F9)/(F6+F8+F9)</f>
         <v>5</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24">
+        <f>F6+F8+F9</f>
+        <v>133</v>
+      </c>
+      <c r="H24" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="24">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="23">
         <v>2</v>
       </c>
       <c r="E25">
@@ -1139,54 +1190,66 @@
         <f>(E7*F7+E10*F10)/(F7+F10)</f>
         <v>5</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25">
+        <f>F7+F10</f>
+        <v>95</v>
+      </c>
+      <c r="H25" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="29">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>F11</f>
         <v>13</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="30">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="30">
+      <c r="H26" s="29">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="33">
-        <v>2</v>
-      </c>
-      <c r="E27" s="36">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="32">
+        <v>2</v>
+      </c>
+      <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
         <f>(E13*F13+E15*F15)/(F13+F15)</f>
         <v>1.6565656565656566</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G27">
+        <f>F13+F15</f>
+        <v>99</v>
+      </c>
+      <c r="H27" s="34">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: explore weighting scenarios
The Excel file explores various weighting schemes and aggregate results from a simulated dataset.
</commit_message>
<xml_diff>
--- a/tests/test-data/weighted-mean-inputs.xlsx
+++ b/tests/test-data/weighted-mean-inputs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\household-size\tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD39A90E-010C-4F95-8260-42B42382918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D7EA0-7472-4F66-94DB-5E2862C3EAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5630" yWindow="160" windowWidth="11300" windowHeight="14090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Weighted Averages" sheetId="1" r:id="rId1"/>
+    <sheet name="Mean household size" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
   <si>
     <t>HHINCOME_bucket</t>
   </si>
@@ -132,6 +155,42 @@
   </si>
   <si>
     <t>aian</t>
+  </si>
+  <si>
+    <t>mean_hh_size_method1</t>
+  </si>
+  <si>
+    <t>mean_hh_size_method2</t>
+  </si>
+  <si>
+    <t>HHWT</t>
+  </si>
+  <si>
+    <t>mean hh size person method</t>
+  </si>
+  <si>
+    <t>mean hh size hh method</t>
+  </si>
+  <si>
+    <t>hhwt</t>
+  </si>
+  <si>
+    <t>Household ID</t>
+  </si>
+  <si>
+    <t>household id</t>
+  </si>
+  <si>
+    <t>numprec</t>
+  </si>
+  <si>
+    <t>mean hh size revised person method</t>
+  </si>
+  <si>
+    <t>PERWT/NUMPREC</t>
+  </si>
+  <si>
+    <t>This one is incorrect vv</t>
   </si>
 </sst>
 </file>
@@ -326,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -362,6 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1253,6 +1313,698 @@
         <v>7</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <f>SUMPRODUCT(F21:F27,G21:G27)/SUM(G21:G27)</f>
+        <v>3.1706539074960127</v>
+      </c>
+      <c r="C31" cm="1">
+        <f t="array" ref="C31">SUMPRODUCT(F3:F17*E3:E17)/SUM(F3:F17)</f>
+        <v>3.1706539074960127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D75B02A-9078-40E4-92A4-2DC67CE6542C}">
+  <dimension ref="A1:J30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="22.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <f>F3/E3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="35">
+        <v>1</v>
+      </c>
+      <c r="J3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G17" si="0">F4/E4</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="35">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="35">
+        <v>1</v>
+      </c>
+      <c r="J5" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="19">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="35">
+        <v>2</v>
+      </c>
+      <c r="J6" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="35">
+        <v>2</v>
+      </c>
+      <c r="J7" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="21">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="35">
+        <v>2</v>
+      </c>
+      <c r="J8" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="21">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="35">
+        <v>2</v>
+      </c>
+      <c r="J9" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="25">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="35">
+        <v>2</v>
+      </c>
+      <c r="J10" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="29">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>3</v>
+      </c>
+      <c r="J11" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="13">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="35">
+        <v>4</v>
+      </c>
+      <c r="J12" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="32">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="35">
+        <v>5</v>
+      </c>
+      <c r="J13" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="17">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="35">
+        <v>5</v>
+      </c>
+      <c r="J14" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="31">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+      <c r="I15" s="35">
+        <v>6</v>
+      </c>
+      <c r="J15" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="35">
+        <v>7</v>
+      </c>
+      <c r="J16" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="15">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="35">
+        <v>7</v>
+      </c>
+      <c r="J17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B30" cm="1">
+        <f t="array" ref="B30">SUMPRODUCT(E3:E17*F3:F17)/SUM(F3:F17)</f>
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f>SUMPRODUCT(B20:B26,C20:C26)/SUM(C20:C26)</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="D30" cm="1">
+        <f t="array" ref="D30">SUMPRODUCT(E3:E17*G3:G17)/SUM(G3:G17)</f>
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>